<commit_message>
replaced example worksheet payroll with timesheet payroll updated version to 0.9.0-beta.6
</commit_message>
<xml_diff>
--- a/Examples/SimplePayroll/Payroll.Lookups.xlsx
+++ b/Examples/SimplePayroll/Payroll.Lookups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\Examples\SimplePayroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37B0E7F-E9E7-428E-8F0E-ABE8DB1FFD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72A0BB8-1EF7-4337-81A7-0DB6C10EF782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
   <si>
-    <t>ASON Payroll Excel Import</t>
-  </si>
-  <si>
     <t>CaseFieldName</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Shared Lookup with name &lt;Name&gt;</t>
+  </si>
+  <si>
+    <t>Payroll Engine Excel Import</t>
   </si>
 </sst>
 </file>
@@ -742,26 +742,26 @@
   </sheetPr>
   <dimension ref="B1:I46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="2.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="8.5500000000000007" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -771,514 +771,514 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:9" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>66</v>
-      </c>
       <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>66</v>
-      </c>
       <c r="D21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="7" t="s">
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="C35" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="D41" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="D46" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1306,52 +1306,52 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="19.7265625" style="27"/>
+    <col min="6" max="6" width="19.77734375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
-        <v>41</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="25">
         <v>50</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="27">
         <v>44944</v>
@@ -1361,21 +1361,21 @@
       </c>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="25">
         <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="25">
         <v>0</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="27">
         <v>44944</v>
@@ -1385,21 +1385,21 @@
       </c>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="25">
         <v>2</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="25">
         <v>0</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="27">
         <v>44944</v>
@@ -1409,21 +1409,21 @@
       </c>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="25">
         <v>2</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="25">
         <v>50</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="27">
         <v>44944</v>
@@ -1433,21 +1433,21 @@
       </c>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="25">
         <v>2</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="25">
         <v>50</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="27">
         <v>44944</v>
@@ -1471,33 +1471,33 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.7265625" style="27"/>
+    <col min="2" max="2" width="19.77734375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>8000</v>
       </c>
@@ -1508,13 +1508,13 @@
         <v>8000</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <v>9464</v>
       </c>
@@ -1525,13 +1525,13 @@
         <v>9464</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="24">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>9470</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>9470</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="24">
         <v>1</v>

</xml_diff>